<commit_message>
Add database file (in xlsx)
</commit_message>
<xml_diff>
--- a/examples/chains.comp.xlsx
+++ b/examples/chains.comp.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2846" uniqueCount="435">
   <si>
     <t xml:space="preserve">select</t>
   </si>
@@ -751,6 +751,585 @@
   </si>
   <si>
     <t xml:space="preserve">b411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c461</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c541</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c591</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c611</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">morph2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">morph3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gpcrmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y013</t>
   </si>
 </sst>
 </file>
@@ -865,7 +1444,7 @@
       <selection pane="topLeft" activeCell="B86" activeCellId="0" sqref="B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.37"/>
@@ -3826,7 +4405,7 @@
   <autoFilter ref="A1:K86"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3840,13 +4419,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K193"/>
+  <dimension ref="A1:K379"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E193" activeCellId="0" sqref="E193"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A354" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G377" activeCellId="0" sqref="G377"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.37"/>
@@ -8279,13 +8858,2628 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E193" s="1"/>
+      <c r="A193" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C193" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C194" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C195" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="C197" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C198" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C204" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C211" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="C216" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B220" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="C220" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C221" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C222" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B224" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C224" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="C225" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B226" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C226" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B229" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C229" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="C230" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B231" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C231" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B232" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C232" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C234" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B235" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C235" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C236" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C237" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="C238" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B239" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="C239" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B240" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="C240" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C241" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B242" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C242" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B243" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B244" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="C244" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B245" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C245" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B246" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B247" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B248" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B249" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B250" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B251" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="C251" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B252" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="C252" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B253" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="C253" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B254" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C254" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B255" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="C255" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B256" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="C256" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B257" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="C257" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B258" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C258" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B259" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="C259" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B260" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C260" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B261" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="C261" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="C262" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C264" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B265" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="C265" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B266" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="C266" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B267" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="C267" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B268" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="C268" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B269" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="C269" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B270" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="C270" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B271" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="C271" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="C272" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B273" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="C273" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B274" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C274" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="C275" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B276" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="C276" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B277" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="C277" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C278" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B279" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="C279" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B280" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="C280" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B281" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="C281" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B282" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="C282" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B283" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="C283" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B284" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="C284" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B285" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="C285" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E285" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="C286" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E286" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B287" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="C287" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E287" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B288" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="C288" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E288" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B289" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="C289" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E289" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B290" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="C290" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E290" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B291" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="C291" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E291" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B292" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="C292" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E292" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B293" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="C293" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E293" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B294" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C294" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E294" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B295" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="C295" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E295" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B296" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="C296" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E296" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B297" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C297" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E297" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B298" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="C298" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E298" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B299" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="C299" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E299" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B300" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="C300" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E300" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B301" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="C301" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E301" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B302" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="C302" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E302" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B303" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="C303" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E303" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B304" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="C304" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E304" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B305" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C305" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E305" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="C306" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E306" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B307" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="C307" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E307" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B308" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C308" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E308" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B309" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="C309" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E309" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B310" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C310" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E310" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B311" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="C311" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E311" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B312" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="C312" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E312" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B313" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="C313" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E313" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B314" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="C314" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E314" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B315" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="C315" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E315" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B316" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C316" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E316" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B317" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="C317" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E317" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B318" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C318" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E318" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B319" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="C319" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E319" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B320" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C320" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E320" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B321" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="C321" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E321" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B322" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="C322" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E322" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B323" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="C323" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E323" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B324" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="C324" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E324" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B325" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="C325" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E325" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B326" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="C326" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E326" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B327" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="C327" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E327" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B328" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E328" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B329" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="C329" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E329" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B330" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="C330" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E330" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B331" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C331" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E331" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B332" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E332" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B333" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="C333" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E333" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B334" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E334" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B335" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="C335" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E335" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B336" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C336" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E336" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B337" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E337" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B338" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="C338" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E338" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B339" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E339" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B340" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="C340" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E340" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B341" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="C341" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E341" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B342" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E342" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B343" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="C343" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E343" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B344" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C344" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E344" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B345" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="C345" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E345" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B346" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="C346" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E346" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B347" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="C347" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E347" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B348" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C348" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E348" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B349" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="C349" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E349" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B350" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="C350" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E350" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B351" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="C351" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E351" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B352" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="C352" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E352" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B353" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="C353" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E353" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B354" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="C354" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E354" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B355" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C355" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E355" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B356" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="C356" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E356" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B357" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="C357" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E357" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B358" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C358" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E358" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B359" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="C359" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E359" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B360" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="C360" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E360" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B361" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="C361" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E361" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B362" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="C362" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E362" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B363" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="C363" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E363" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B364" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="C364" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E364" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B365" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="C365" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E365" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B366" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="C366" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E366" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B367" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="C367" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E367" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B368" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="C368" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E368" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B369" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="C369" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E369" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B370" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C370" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E370" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B371" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="C371" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E371" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B372" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="C372" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E372" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B373" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="C373" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E373" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B374" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="C374" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E374" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B375" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="C375" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E375" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B376" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C376" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E376" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B377" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C377" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E377" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B378" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C378" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E378" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B379" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="C379" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E379" s="0" t="s">
+        <v>267</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K86"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>